<commit_message>
features seem to be calculated soundly
</commit_message>
<xml_diff>
--- a/pepfeature/AAdescriptors.xlsx
+++ b/pepfeature/AAdescriptors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xbox_\Documents\GitHub\epifeature\pepfeature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7DCAFB-DC5C-4E29-BFE9-BD9D8C6537CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7028CCFD-A7F2-4F5B-93A0-4317C95EE846}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="731" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -340,7 +340,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -353,6 +353,13 @@
       <color rgb="FF172B4D"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -372,15 +379,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{E8541B58-92BA-4910-A137-4C35EAE886C7}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3916,8 +3926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U6" sqref="B6:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4254,64 +4264,64 @@
       <c r="A6" t="s">
         <v>56</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>-0.39</v>
       </c>
-      <c r="C6">
-        <v>-0.39</v>
-      </c>
-      <c r="D6">
-        <v>-0.39</v>
-      </c>
-      <c r="E6">
-        <v>-0.39</v>
-      </c>
-      <c r="F6">
-        <v>-0.39</v>
-      </c>
-      <c r="G6">
-        <v>-0.39</v>
-      </c>
-      <c r="H6">
-        <v>-0.39</v>
-      </c>
-      <c r="I6">
-        <v>-0.39</v>
-      </c>
-      <c r="J6">
-        <v>-0.39</v>
-      </c>
-      <c r="K6">
-        <v>-0.39</v>
-      </c>
-      <c r="L6">
-        <v>-0.39</v>
-      </c>
-      <c r="M6">
-        <v>-0.39</v>
-      </c>
-      <c r="N6">
-        <v>-0.39</v>
-      </c>
-      <c r="O6">
-        <v>-0.39</v>
-      </c>
-      <c r="P6">
-        <v>-0.39</v>
-      </c>
-      <c r="Q6">
-        <v>-0.39</v>
-      </c>
-      <c r="R6">
-        <v>-0.39</v>
-      </c>
-      <c r="S6">
+      <c r="C6" s="2">
+        <v>3.27</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="E6" s="2">
+        <v>-2.14</v>
+      </c>
+      <c r="F6" s="2">
+        <v>-0.49</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-0.31</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="I6" s="2">
+        <v>-0.34</v>
+      </c>
+      <c r="J6" s="2">
+        <v>-1.23</v>
+      </c>
+      <c r="K6" s="2">
+        <v>-1.7</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="N6" s="2">
+        <v>-3.22</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="P6" s="2">
+        <v>1.67</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="R6" s="2">
+        <v>1.06</v>
+      </c>
+      <c r="S6" s="2">
         <v>0.06</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="2">
         <v>-1.08</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="2">
         <v>-0.06</v>
       </c>
     </row>

</xml_diff>